<commit_message>
Updated task list - algorithm about topic search engine has been added.
</commit_message>
<xml_diff>
--- a/task_list.xlsx
+++ b/task_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Task ID</t>
   </si>
@@ -129,9 +129,6 @@
                3. Откритата фраза. (Връща празен стринг ако не открие фразата)</t>
   </si>
   <si>
-    <t xml:space="preserve">6. Функция </t>
-  </si>
-  <si>
     <t>Написване на клас project</t>
   </si>
   <si>
@@ -141,6 +138,12 @@
 3. Факултетен номер (String)
 4. Университет (тип String)
 5. Сложност (Enum)</t>
+  </si>
+  <si>
+    <t>6. Функция която връща фраза, съдържаща думи</t>
+  </si>
+  <si>
+    <t>Информацията която се извлича за автор, факултетен номер и Университет се записва в структура (клас) със съответните полета и се замества в текста извлечен от първата страница на всеки документ с \n (символа за нов ред). След това в този текст се търсят ключови фрази "на тема", "тема на проекта", "тема на курсовия проект", "тема на курсовата работа", "тема на дипломната работа", "тема на преддипломния проект", "тема на преддипломната работа" и др И се извлича всичко след тях докато не се стигне до следните стоп фрази "\n\n" (!Независимо колко интервала има между тях - използвай невронната мрежа - PosTag), "по дисциплината", "разработен за" и др.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +176,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -203,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +236,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -694,80 +704,85 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C5" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="42" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>4</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="3" t="s">
+    <row r="45" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="3" t="s">
+    <row r="46" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="C10" s="6" t="s">
+    <row r="47" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="C47" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="C11" s="6" t="s">
+    <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="C48" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="C12" s="6" t="s">
+    <row r="49" spans="3:3" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="C49" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="6" t="s">
-        <v>25</v>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="F1:F1005">

</xml_diff>